<commit_message>
Creating new bigger dataset
</commit_message>
<xml_diff>
--- a/model notes.xlsx
+++ b/model notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Model</t>
   </si>
@@ -24,63 +24,12 @@
     <t>Server</t>
   </si>
   <si>
-    <t>0.0.4.09</t>
-  </si>
-  <si>
-    <t>EC2</t>
-  </si>
-  <si>
-    <t>0.0.0.21</t>
-  </si>
-  <si>
     <t>i8</t>
   </si>
   <si>
-    <t>Tr5</t>
-  </si>
-  <si>
-    <t>Cv5</t>
-  </si>
-  <si>
-    <t>Tr10</t>
-  </si>
-  <si>
-    <t>Cv10</t>
-  </si>
-  <si>
-    <t>Tr15</t>
-  </si>
-  <si>
-    <t>Cv15</t>
-  </si>
-  <si>
-    <t>Tr20</t>
-  </si>
-  <si>
-    <t>Cv20</t>
-  </si>
-  <si>
-    <t>CR10</t>
-  </si>
-  <si>
-    <t>CP10</t>
-  </si>
-  <si>
-    <t>CR20</t>
-  </si>
-  <si>
-    <t>CP20</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Trained fast, accuracy went up quickly but precision and recall are lagging</t>
-  </si>
-  <si>
-    <t>0.0.0.22</t>
-  </si>
-  <si>
     <t>i7</t>
   </si>
   <si>
@@ -102,13 +51,40 @@
     <t>Min/Ep</t>
   </si>
   <si>
-    <t>0.0.1.02</t>
-  </si>
-  <si>
-    <t>Looked good through epoch 9, then accuracy started to plummet</t>
-  </si>
-  <si>
-    <t>0.0.4.11</t>
+    <t>1.0.1.39n</t>
+  </si>
+  <si>
+    <t>Epochs</t>
+  </si>
+  <si>
+    <t>Test Acc</t>
+  </si>
+  <si>
+    <t>Test Re</t>
+  </si>
+  <si>
+    <t>CvAcc</t>
+  </si>
+  <si>
+    <t>TrAcc</t>
+  </si>
+  <si>
+    <t>TrPr</t>
+  </si>
+  <si>
+    <t>CvPr</t>
+  </si>
+  <si>
+    <t>TrRe</t>
+  </si>
+  <si>
+    <t>CvRe</t>
+  </si>
+  <si>
+    <t>Good results, but CV results volatile</t>
+  </si>
+  <si>
+    <t>1.0.0.28</t>
   </si>
 </sst>
 </file>
@@ -460,11 +436,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -479,15 +455,14 @@
     <col min="11" max="11" width="7.86328125" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
     <col min="13" max="14" width="8.1328125" customWidth="1"/>
-    <col min="15" max="15" width="8.3984375" customWidth="1"/>
-    <col min="16" max="16" width="4" customWidth="1"/>
-    <col min="17" max="17" width="8.3984375" customWidth="1"/>
-    <col min="18" max="18" width="5.33203125" customWidth="1"/>
-    <col min="19" max="23" width="8.6640625" customWidth="1"/>
-    <col min="24" max="24" width="5.33203125" customWidth="1"/>
+    <col min="15" max="15" width="4" customWidth="1"/>
+    <col min="16" max="16" width="8.3984375" customWidth="1"/>
+    <col min="17" max="17" width="5.33203125" customWidth="1"/>
+    <col min="18" max="22" width="8.6640625" customWidth="1"/>
+    <col min="23" max="23" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,442 +471,323 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="S1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E2">
+        <v>0.99350000000000005</v>
+      </c>
+      <c r="F2">
+        <v>0.96809999999999996</v>
+      </c>
+      <c r="G2">
+        <v>0.99709999999999999</v>
+      </c>
+      <c r="H2">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="I2">
+        <v>0.95750000000000002</v>
+      </c>
+      <c r="K2">
+        <v>47</v>
+      </c>
+      <c r="M2">
+        <v>0.99350000000000005</v>
+      </c>
+      <c r="N2">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="X2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>0.88819999999999999</v>
-      </c>
-      <c r="E2">
-        <v>0.87309999999999999</v>
-      </c>
-      <c r="F2">
-        <v>0.95309999999999995</v>
-      </c>
-      <c r="G2">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="H2">
-        <v>0.55530000000000002</v>
-      </c>
-      <c r="I2">
-        <v>0.7238</v>
-      </c>
-      <c r="Q2">
-        <v>25</v>
-      </c>
-      <c r="S2" s="2">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="T2" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="V2" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="W2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
       <c r="D3">
-        <v>0.92190000000000005</v>
+        <v>0.99639999999999995</v>
       </c>
       <c r="E3">
-        <v>0.81789999999999996</v>
+        <v>0.99039999999999995</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0.98219999999999996</v>
       </c>
       <c r="G3">
-        <v>0.62680000000000002</v>
+        <v>0.98850000000000005</v>
       </c>
       <c r="H3">
-        <v>0.67820000000000003</v>
+        <v>0.996</v>
       </c>
       <c r="I3">
-        <v>0.60460000000000003</v>
-      </c>
-      <c r="J3">
-        <v>0.98440000000000005</v>
+        <v>0.94369999999999998</v>
       </c>
       <c r="K3">
-        <v>0.83079999999999998</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="M3">
-        <v>0.97040000000000004</v>
+        <v>0.99029999999999996</v>
       </c>
       <c r="N3">
-        <v>0.76819999999999999</v>
-      </c>
-      <c r="O3">
-        <v>0.73140000000000005</v>
-      </c>
-      <c r="Q3">
-        <v>7</v>
-      </c>
+        <v>0.94310000000000005</v>
+      </c>
+      <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="Y3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4">
-        <v>0.89059999999999995</v>
-      </c>
-      <c r="E4">
-        <v>0.89849999999999997</v>
-      </c>
-      <c r="F4">
-        <v>0.98440000000000005</v>
-      </c>
-      <c r="G4">
-        <v>0.90649999999999997</v>
-      </c>
-      <c r="H4">
-        <v>0.57889999999999997</v>
-      </c>
-      <c r="I4">
-        <v>0.64100000000000001</v>
-      </c>
-      <c r="J4">
-        <v>0.96879999999999999</v>
-      </c>
-      <c r="K4">
-        <v>0.89549999999999996</v>
-      </c>
-      <c r="L4">
-        <v>0.85940000000000005</v>
-      </c>
-      <c r="M4">
-        <v>0.90390000000000004</v>
-      </c>
-      <c r="N4">
-        <v>0.68669999999999998</v>
-      </c>
-      <c r="O4">
-        <v>0.7036</v>
-      </c>
-      <c r="Q4">
-        <v>7</v>
-      </c>
-      <c r="S4" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="T4" s="2">
-        <v>1.5E-3</v>
-      </c>
-      <c r="U4" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="V4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="W4" s="2">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q5">
-        <v>11</v>
-      </c>
-      <c r="S5" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="T5" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="U5" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="V5" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="W5" s="2">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q6">
-        <v>30</v>
-      </c>
-      <c r="S6" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="T6" s="2">
-        <v>1.5E-3</v>
-      </c>
-      <c r="U6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="V6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="W6" s="2">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R16" s="2"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-    </row>
-    <row r="17" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-    </row>
-    <row r="18" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-    </row>
-    <row r="19" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R19" s="2"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-    </row>
-    <row r="20" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R20" s="2"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-    </row>
-    <row r="21" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-    </row>
-    <row r="22" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-    </row>
-    <row r="23" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
-    </row>
-    <row r="24" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R24" s="2"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-    </row>
-    <row r="25" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-    </row>
-    <row r="26" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
-    </row>
-    <row r="27" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
-    </row>
-    <row r="28" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R28" s="2"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
-    </row>
-    <row r="29" spans="19:23" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="18:22" x14ac:dyDescent="0.45">
+      <c r="R29" s="2"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Some final metrics and results
</commit_message>
<xml_diff>
--- a/model notes.xlsx
+++ b/model notes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="140">
   <si>
     <t>Model</t>
   </si>
@@ -414,10 +414,31 @@
     <t>1.0.0.35b.98</t>
   </si>
   <si>
-    <t>Continuing to train for 10 epochs with online data aug</t>
-  </si>
-  <si>
     <t>Stopped training after 3 additional epochs as results dropped</t>
+  </si>
+  <si>
+    <t>Training for extra 5 epochs</t>
+  </si>
+  <si>
+    <t>Training for extra 10 epochs</t>
+  </si>
+  <si>
+    <t>vgg_16.3.06b.9</t>
+  </si>
+  <si>
+    <t>Retraining VGG with online data aug and proper xe weight</t>
+  </si>
+  <si>
+    <t>Continuing to train for extra 5 epochs</t>
+  </si>
+  <si>
+    <t>Retraining to tune hyperparameters</t>
+  </si>
+  <si>
+    <t>Training to tune hyperparameters</t>
+  </si>
+  <si>
+    <t>Continuing to train VGG for extra 10 epochs, with lowered xe weight</t>
   </si>
 </sst>
 </file>
@@ -503,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -514,6 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,11 +837,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z62"/>
+  <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65:A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4726,7 +4748,7 @@
         <v>11</v>
       </c>
       <c r="Z58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.45">
@@ -4783,7 +4805,7 @@
       </c>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B60" t="s">
@@ -4807,19 +4829,52 @@
       <c r="H60">
         <v>1</v>
       </c>
+      <c r="J60">
+        <v>0.91190000000000004</v>
+      </c>
+      <c r="K60">
+        <v>0.68630000000000002</v>
+      </c>
+      <c r="L60">
+        <v>0.78110000000000002</v>
+      </c>
+      <c r="M60">
+        <v>0.51090000000000002</v>
+      </c>
+      <c r="N60">
+        <v>0.66679999999999995</v>
+      </c>
+      <c r="O60">
+        <v>0.34510000000000002</v>
+      </c>
       <c r="Q60">
         <v>20</v>
       </c>
+      <c r="S60">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="T60">
+        <v>0.96289999999999998</v>
+      </c>
+      <c r="U60">
+        <v>0.92410000000000003</v>
+      </c>
+      <c r="V60">
+        <v>0.65910000000000002</v>
+      </c>
       <c r="X60">
         <v>9</v>
       </c>
+      <c r="Z60" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A61" s="2" t="s">
-        <v>123</v>
+      <c r="A61" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="B61" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C61">
         <v>32</v>
@@ -4831,57 +4886,60 @@
         <v>38</v>
       </c>
       <c r="F61">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G61">
         <v>1</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61">
-        <v>0.91059999999999997</v>
+        <v>0.94069999999999998</v>
       </c>
       <c r="K61">
-        <v>0.8659</v>
+        <v>0.97019999999999995</v>
       </c>
       <c r="L61">
-        <v>0.66320000000000001</v>
+        <v>0.75449999999999995</v>
       </c>
       <c r="M61">
-        <v>0.56379999999999997</v>
+        <v>0.94289999999999996</v>
       </c>
       <c r="N61">
-        <v>0.94430000000000003</v>
+        <v>0.94540000000000002</v>
       </c>
       <c r="O61">
-        <v>0.86429999999999996</v>
+        <v>0.87429999999999997</v>
       </c>
       <c r="Q61">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="S61">
-        <v>0.85799999999999998</v>
+        <v>0.96419999999999995</v>
       </c>
       <c r="T61">
-        <v>0.88480000000000003</v>
+        <v>0.87450000000000006</v>
       </c>
       <c r="U61">
-        <v>0.71560000000000001</v>
+        <v>0.75849999999999995</v>
       </c>
       <c r="V61">
-        <v>0.89049999999999996</v>
+        <v>0.8921</v>
       </c>
       <c r="X61">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A62" s="2" t="s">
-        <v>123</v>
+      <c r="A62" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C62">
         <v>32</v>
@@ -4901,11 +4959,345 @@
       <c r="H62">
         <v>1</v>
       </c>
+      <c r="J62">
+        <v>0.95579999999999998</v>
+      </c>
+      <c r="K62">
+        <v>0.97160000000000002</v>
+      </c>
+      <c r="L62">
+        <v>0.80759999999999998</v>
+      </c>
+      <c r="M62">
+        <v>0.91839999999999999</v>
+      </c>
+      <c r="N62">
+        <v>0.96560000000000001</v>
+      </c>
+      <c r="O62">
+        <v>0.91020000000000001</v>
+      </c>
       <c r="Q62">
+        <v>5</v>
+      </c>
+      <c r="S62">
+        <v>0.95709999999999995</v>
+      </c>
+      <c r="T62">
+        <v>0.9012</v>
+      </c>
+      <c r="U62">
+        <v>0.88019999999999998</v>
+      </c>
+      <c r="V62">
+        <v>0.81730000000000003</v>
+      </c>
+      <c r="X62">
         <v>10</v>
       </c>
       <c r="Z62" t="s">
-        <v>131</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A63" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>32</v>
+      </c>
+      <c r="D63">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>38</v>
+      </c>
+      <c r="F63">
+        <v>6</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0.91059999999999997</v>
+      </c>
+      <c r="K63">
+        <v>0.8659</v>
+      </c>
+      <c r="L63">
+        <v>0.66320000000000001</v>
+      </c>
+      <c r="M63">
+        <v>0.56379999999999997</v>
+      </c>
+      <c r="N63">
+        <v>0.94430000000000003</v>
+      </c>
+      <c r="O63">
+        <v>0.86429999999999996</v>
+      </c>
+      <c r="Q63">
+        <v>20</v>
+      </c>
+      <c r="S63">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="T63">
+        <v>0.88480000000000003</v>
+      </c>
+      <c r="U63">
+        <v>0.71560000000000001</v>
+      </c>
+      <c r="V63">
+        <v>0.89049999999999996</v>
+      </c>
+      <c r="X63">
+        <v>11</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="10">
+        <v>32</v>
+      </c>
+      <c r="D64" s="10">
+        <v>9</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F64" s="10">
+        <v>5</v>
+      </c>
+      <c r="G64" s="10">
+        <v>1</v>
+      </c>
+      <c r="H64" s="10">
+        <v>1</v>
+      </c>
+      <c r="J64" s="10">
+        <v>0.94220000000000004</v>
+      </c>
+      <c r="K64" s="10">
+        <v>0.93759999999999999</v>
+      </c>
+      <c r="L64" s="10">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="M64" s="10">
+        <v>0.79220000000000002</v>
+      </c>
+      <c r="N64" s="10">
+        <v>0.95369999999999999</v>
+      </c>
+      <c r="O64" s="10">
+        <v>0.84830000000000005</v>
+      </c>
+      <c r="Q64" s="10">
+        <v>15</v>
+      </c>
+      <c r="S64">
+        <v>0.89629999999999999</v>
+      </c>
+      <c r="T64">
+        <v>0.91410000000000002</v>
+      </c>
+      <c r="U64">
+        <v>0.83609999999999995</v>
+      </c>
+      <c r="V64">
+        <v>0.83689999999999998</v>
+      </c>
+      <c r="X64" s="10">
+        <v>10</v>
+      </c>
+      <c r="Z64" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A65" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="10">
+        <v>32</v>
+      </c>
+      <c r="D65" s="10">
+        <v>9</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F65" s="10">
+        <v>6</v>
+      </c>
+      <c r="G65" s="10">
+        <v>1</v>
+      </c>
+      <c r="H65" s="10">
+        <v>1</v>
+      </c>
+      <c r="J65" s="10">
+        <v>0.92069999999999996</v>
+      </c>
+      <c r="K65" s="10">
+        <v>0.86329999999999996</v>
+      </c>
+      <c r="L65" s="10">
+        <v>0.69110000000000005</v>
+      </c>
+      <c r="M65" s="10">
+        <v>0.62560000000000004</v>
+      </c>
+      <c r="N65" s="10">
+        <v>0.94850000000000001</v>
+      </c>
+      <c r="O65" s="10">
+        <v>0.91849999999999998</v>
+      </c>
+      <c r="Q65" s="10">
+        <v>20</v>
+      </c>
+      <c r="S65">
+        <v>0.84219999999999995</v>
+      </c>
+      <c r="T65">
+        <v>0.94950000000000001</v>
+      </c>
+      <c r="U65">
+        <v>0.49149999999999999</v>
+      </c>
+      <c r="V65">
+        <v>0.98280000000000001</v>
+      </c>
+      <c r="X65" s="10">
+        <v>15</v>
+      </c>
+      <c r="Z65" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A66" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="10">
+        <v>32</v>
+      </c>
+      <c r="D66" s="10">
+        <v>9</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F66" s="10">
+        <v>5</v>
+      </c>
+      <c r="G66" s="10">
+        <v>1</v>
+      </c>
+      <c r="H66" s="10">
+        <v>1</v>
+      </c>
+      <c r="J66" s="10">
+        <v>0.94650000000000001</v>
+      </c>
+      <c r="K66" s="10">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="L66" s="10">
+        <v>0.77390000000000003</v>
+      </c>
+      <c r="M66" s="10">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="N66" s="10">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="O66" s="10">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="Q66" s="10">
+        <v>10</v>
+      </c>
+      <c r="S66">
+        <v>0.81379999999999997</v>
+      </c>
+      <c r="T66">
+        <v>0.98839999999999995</v>
+      </c>
+      <c r="U66">
+        <v>0.43569999999999998</v>
+      </c>
+      <c r="V66">
+        <v>0.97970000000000002</v>
+      </c>
+      <c r="X66" s="10">
+        <v>15</v>
+      </c>
+      <c r="Z66" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A67" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="10">
+        <v>32</v>
+      </c>
+      <c r="D67" s="10">
+        <v>9</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F67" s="10">
+        <v>4</v>
+      </c>
+      <c r="G67" s="10">
+        <v>1</v>
+      </c>
+      <c r="H67" s="10">
+        <v>1</v>
+      </c>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+      <c r="N67" s="10"/>
+      <c r="O67" s="10"/>
+      <c r="Q67" s="10">
+        <v>5</v>
+      </c>
+      <c r="X67" s="10">
+        <v>15</v>
+      </c>
+      <c r="Z67" s="10" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redoing dataset 11 so it will work with whole images
</commit_message>
<xml_diff>
--- a/model notes.xlsx
+++ b/model notes.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="113" windowWidth="23310" windowHeight="9983" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="113" windowWidth="23310" windowHeight="9983" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Eval" sheetId="2" r:id="rId2"/>
-    <sheet name="Whole Image Preds" sheetId="3" r:id="rId3"/>
+    <sheet name="FullImage" sheetId="3" r:id="rId3"/>
     <sheet name="Datasets" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="220">
   <si>
     <t>Model</t>
   </si>
@@ -605,7 +605,82 @@
     <t>101-200</t>
   </si>
   <si>
-    <t>Correct</t>
+    <t>Acc</t>
+  </si>
+  <si>
+    <t>51-100</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>101-150</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>151-200</t>
+  </si>
+  <si>
+    <t>201-250</t>
+  </si>
+  <si>
+    <t>251-300</t>
+  </si>
+  <si>
+    <t>301-322</t>
+  </si>
+  <si>
+    <t>0-100</t>
+  </si>
+  <si>
+    <t>Training for 5 more epochs with lower xe weight</t>
+  </si>
+  <si>
+    <t>251-292</t>
+  </si>
+  <si>
+    <t>201-300</t>
+  </si>
+  <si>
+    <t>301-362</t>
+  </si>
+  <si>
+    <t>One negative was right on edge so probably cropped out</t>
+  </si>
+  <si>
+    <t>Howtek</t>
+  </si>
+  <si>
+    <t>301-400</t>
+  </si>
+  <si>
+    <t>401-500</t>
+  </si>
+  <si>
+    <t>501-551</t>
+  </si>
+  <si>
+    <t>Training more with even lower xe weight and raised contrast</t>
+  </si>
+  <si>
+    <t>Howtek b.10</t>
+  </si>
+  <si>
+    <t>0-200</t>
+  </si>
+  <si>
+    <t>201-400</t>
+  </si>
+  <si>
+    <t>401-551</t>
+  </si>
+  <si>
+    <t>CalcTest b.10</t>
+  </si>
+  <si>
+    <t>201-291</t>
   </si>
 </sst>
 </file>
@@ -1004,11 +1079,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z87"/>
+  <dimension ref="A1:Z89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O88" sqref="O88"/>
+      <selection pane="bottomLeft" activeCell="C71" sqref="C71:C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6687,6 +6762,133 @@
         <v>15</v>
       </c>
     </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A88" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C88" s="9">
+        <v>32</v>
+      </c>
+      <c r="D88" s="9">
+        <v>10</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F88" s="9">
+        <v>7</v>
+      </c>
+      <c r="G88" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H88" s="9">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>0.98040000000000005</v>
+      </c>
+      <c r="K88">
+        <v>0.97919999999999996</v>
+      </c>
+      <c r="L88">
+        <v>0.878</v>
+      </c>
+      <c r="M88">
+        <v>0.89490000000000003</v>
+      </c>
+      <c r="N88">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="O88">
+        <v>0.95209999999999995</v>
+      </c>
+      <c r="Q88" s="9">
+        <v>5</v>
+      </c>
+      <c r="S88">
+        <v>0.97170000000000001</v>
+      </c>
+      <c r="T88">
+        <v>0.94830000000000003</v>
+      </c>
+      <c r="U88">
+        <v>0.63780000000000003</v>
+      </c>
+      <c r="V88">
+        <v>0.90469999999999995</v>
+      </c>
+      <c r="X88">
+        <v>15</v>
+      </c>
+      <c r="Z88" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A89" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C89" s="9">
+        <v>32</v>
+      </c>
+      <c r="D89" s="9">
+        <v>10</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F89" s="9">
+        <v>6</v>
+      </c>
+      <c r="G89" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="H89" s="9">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <v>0.98429999999999995</v>
+      </c>
+      <c r="K89">
+        <v>0.97940000000000005</v>
+      </c>
+      <c r="L89">
+        <v>0.90059999999999996</v>
+      </c>
+      <c r="M89">
+        <v>0.90110000000000001</v>
+      </c>
+      <c r="N89">
+        <v>0.98829999999999996</v>
+      </c>
+      <c r="O89">
+        <v>0.94610000000000005</v>
+      </c>
+      <c r="Q89" s="9">
+        <v>5</v>
+      </c>
+      <c r="S89">
+        <v>0.96719999999999995</v>
+      </c>
+      <c r="T89">
+        <v>0.88780000000000003</v>
+      </c>
+      <c r="U89">
+        <v>0.80020000000000002</v>
+      </c>
+      <c r="V89">
+        <v>0.87039999999999995</v>
+      </c>
+      <c r="Z89" t="s">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E60"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7291,11 +7493,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7366,14 +7568,23 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="G2">
         <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.48</v>
+      </c>
+      <c r="I2">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="J2">
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="K2">
         <f>(D2-F2)/D2</f>
-        <v>0.55172413793103448</v>
+        <v>0.60254083484573506</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
@@ -7393,23 +7604,23 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="G3">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="H3">
-        <v>0.97319999999999995</v>
+        <v>0.98519999999999996</v>
       </c>
       <c r="I3">
         <v>0.99990000000000001</v>
       </c>
       <c r="J3">
-        <v>3.6600000000000001E-2</v>
+        <v>0.54510000000000003</v>
       </c>
       <c r="K3">
         <f>F3/D3</f>
-        <v>0.96907216494845361</v>
+        <v>0.97938144329896903</v>
       </c>
       <c r="L3" t="s">
         <v>172</v>
@@ -7539,6 +7750,24 @@
       <c r="E7" t="s">
         <v>182</v>
       </c>
+      <c r="F7">
+        <v>187</v>
+      </c>
+      <c r="G7">
+        <v>70</v>
+      </c>
+      <c r="H7">
+        <v>0.74490000000000001</v>
+      </c>
+      <c r="I7">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="J7">
+        <v>4.36E-2</v>
+      </c>
+      <c r="K7">
+        <v>0.49419999999999997</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -7574,6 +7803,118 @@
       <c r="K8">
         <f>(D8-F8)/D8</f>
         <v>0.56707317073170727</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>291</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>282</v>
+      </c>
+      <c r="G9">
+        <v>282</v>
+      </c>
+      <c r="H9">
+        <v>0.98740000000000006</v>
+      </c>
+      <c r="I9">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="J9">
+        <v>0.1007</v>
+      </c>
+      <c r="K9">
+        <f>F9/D9</f>
+        <v>0.96907216494845361</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>362</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>352</v>
+      </c>
+      <c r="G10">
+        <v>352</v>
+      </c>
+      <c r="H10">
+        <f>352/362</f>
+        <v>0.97237569060773477</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1E-4</v>
+      </c>
+      <c r="K10">
+        <f>352/362</f>
+        <v>0.97237569060773477</v>
+      </c>
+      <c r="L10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>551</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>284</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.63049999999999995</v>
+      </c>
+      <c r="I11">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="J11">
+        <v>1E-4</v>
+      </c>
+      <c r="K11">
+        <f>(551-284)/551</f>
+        <v>0.48457350272232302</v>
       </c>
     </row>
   </sheetData>
@@ -7584,11 +7925,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7687,12 +8028,23 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
+        <v>9.9</v>
+      </c>
+      <c r="B9">
+        <v>52739</v>
+      </c>
+      <c r="C9">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>55890</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>0.86950000000000005</v>
       </c>
     </row>
@@ -7703,16 +8055,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>186</v>
       </c>
@@ -7726,44 +8078,1049 @@
         <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="J1" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B2">
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>0.46</v>
+      </c>
+      <c r="E2">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="F2">
+        <v>0.80730000000000002</v>
+      </c>
+      <c r="G2">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H2">
+        <v>0.22570000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>0.53059999999999996</v>
+      </c>
+      <c r="E3">
+        <v>0.5333</v>
+      </c>
+      <c r="F3">
+        <v>0.70850000000000002</v>
+      </c>
+      <c r="G3">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H3">
+        <v>0.1071</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>0.53059999999999996</v>
+      </c>
+      <c r="E4">
+        <v>0.60860000000000003</v>
+      </c>
+      <c r="F4">
+        <v>0.73650000000000004</v>
+      </c>
+      <c r="G4">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H4">
+        <v>4.36E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>0.44890000000000002</v>
+      </c>
+      <c r="E5">
+        <v>0.59089999999999998</v>
+      </c>
+      <c r="F5">
+        <v>0.7883</v>
+      </c>
+      <c r="G5">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H5">
+        <v>0.10539999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>0.59179999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.70369999999999999</v>
+      </c>
+      <c r="F6">
+        <v>0.77849999999999997</v>
+      </c>
+      <c r="G6">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="H6">
+        <v>0.1202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>0.32650000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.4</v>
+      </c>
+      <c r="F7">
+        <v>0.7853</v>
+      </c>
+      <c r="G7">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H7">
+        <v>9.2899999999999996E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.57140000000000002</v>
+      </c>
+      <c r="E8">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F8">
+        <v>0.61040000000000005</v>
+      </c>
+      <c r="G8">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="H8">
+        <v>0.2094</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B2:B10)</f>
+        <v>187</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C2:C10)</f>
+        <v>70</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(D2:D10)</f>
+        <v>0.49425714285714284</v>
+      </c>
+      <c r="E12">
+        <f>AVERAGE(E2:E10)</f>
+        <v>0.55758571428571424</v>
+      </c>
+      <c r="F12">
+        <f>AVERAGE(F2:F10)</f>
+        <v>0.74497142857142862</v>
+      </c>
+      <c r="G12">
+        <f>MAX(G2:G10)</f>
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H12">
+        <f>MIN(H2:H10)</f>
+        <v>4.36E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15">
+        <v>49</v>
+      </c>
+      <c r="C15">
+        <v>49</v>
+      </c>
+      <c r="D15">
+        <f>49/50</f>
+        <v>0.98</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0.98170000000000002</v>
+      </c>
+      <c r="G15">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H15">
+        <v>0.2928</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16">
+        <v>47</v>
+      </c>
+      <c r="C16">
+        <v>47</v>
+      </c>
+      <c r="D16">
+        <f>C16/49</f>
+        <v>0.95918367346938771</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0.96079999999999999</v>
+      </c>
+      <c r="G16">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H16">
+        <v>0.1007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17">
+        <v>49</v>
+      </c>
+      <c r="C17">
+        <v>49</v>
+      </c>
+      <c r="D17">
+        <f>49/49</f>
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0.9929</v>
+      </c>
+      <c r="G17">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H17">
+        <v>0.7591</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>199</v>
+      </c>
+      <c r="B18">
+        <v>49</v>
+      </c>
+      <c r="C18">
+        <v>49</v>
+      </c>
+      <c r="D18">
+        <f>49/49</f>
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0.99850000000000005</v>
+      </c>
+      <c r="G18">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H18">
+        <v>0.98550000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>200</v>
+      </c>
+      <c r="B19">
+        <v>48</v>
+      </c>
+      <c r="C19">
+        <v>48</v>
+      </c>
+      <c r="D19">
+        <f>48/49</f>
+        <v>0.97959183673469385</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0.99180000000000001</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0.65500000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>205</v>
+      </c>
+      <c r="B20">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0.99919999999999998</v>
+      </c>
+      <c r="G20">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H20">
+        <v>0.99229999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B25">
+        <f>SUM(B15:B23)</f>
+        <v>282</v>
+      </c>
+      <c r="C25">
+        <f>SUM(C15:C23)</f>
+        <v>282</v>
+      </c>
+      <c r="D25">
+        <f>AVERAGE(D15:D21)</f>
+        <v>0.98646258503401363</v>
+      </c>
+      <c r="E25">
+        <f>AVERAGE(E15:E23)</f>
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f>AVERAGE(F15:F23)</f>
+        <v>0.98748333333333338</v>
+      </c>
+      <c r="G25">
+        <f>MAX(G15:G23)</f>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <f>MIN(H15:H23)</f>
+        <v>0.1007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>203</v>
+      </c>
+      <c r="B28">
+        <v>98</v>
+      </c>
+      <c r="C28">
+        <v>98</v>
+      </c>
+      <c r="D28">
+        <v>0.98</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0.98029999999999995</v>
+      </c>
+      <c r="G28">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H28">
+        <v>5.5500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B29">
+        <v>49</v>
+      </c>
+      <c r="C29">
+        <v>49</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0.99319999999999997</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0.76470000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>199</v>
+      </c>
+      <c r="B30">
+        <v>48</v>
+      </c>
+      <c r="C30">
+        <v>48</v>
+      </c>
+      <c r="D30">
+        <f>48/49</f>
+        <v>0.97959183673469385</v>
+      </c>
+      <c r="E30">
+        <f>48/49</f>
+        <v>0.97959183673469385</v>
+      </c>
+      <c r="F30">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="G30">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H30">
+        <v>0.30880000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>200</v>
+      </c>
+      <c r="B31">
+        <v>49</v>
+      </c>
+      <c r="C31">
+        <v>49</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="G31">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H31">
+        <v>0.99250000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>201</v>
+      </c>
+      <c r="B32">
+        <v>49</v>
+      </c>
+      <c r="C32">
+        <v>49</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0.99929999999999997</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>0.98540000000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33">
+        <v>59</v>
+      </c>
+      <c r="C33">
+        <v>59</v>
+      </c>
+      <c r="D33">
+        <f>59/61</f>
+        <v>0.96721311475409832</v>
+      </c>
+      <c r="E33">
+        <f>59/61</f>
+        <v>0.96721311475409832</v>
+      </c>
+      <c r="F33">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G33">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H33">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B38">
+        <f>SUM(B28:B36)</f>
+        <v>352</v>
+      </c>
+      <c r="C38">
+        <f>SUM(C28:C36)</f>
+        <v>352</v>
+      </c>
+      <c r="D38">
+        <f>AVERAGE(D28:D34)</f>
+        <v>0.98780082524813206</v>
+      </c>
+      <c r="E38">
+        <f>AVERAGE(E28:E36)</f>
+        <v>0.99113415858146536</v>
+      </c>
+      <c r="F38">
+        <f>AVERAGE(F28:F36)</f>
+        <v>0.9885666666666667</v>
+      </c>
+      <c r="G38">
+        <f>MAX(G28:G36)</f>
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <f>MIN(H28:H36)</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>203</v>
+      </c>
+      <c r="B42">
+        <v>29</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <f>(100-B42)/100</f>
+        <v>0.71</v>
+      </c>
+      <c r="E42" t="s">
+        <v>182</v>
+      </c>
+      <c r="F42">
+        <v>0.4541</v>
+      </c>
+      <c r="G42">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H42">
+        <v>8.0000000000000007E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
+      <c r="B43">
+        <v>37</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <f>(100-B43)/100</f>
+        <v>0.63</v>
+      </c>
+      <c r="E43" t="s">
+        <v>182</v>
+      </c>
+      <c r="F43">
+        <v>0.503</v>
+      </c>
+      <c r="G43">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H43">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>206</v>
+      </c>
+      <c r="B44">
+        <v>49</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <f>(100-B44)/100</f>
+        <v>0.51</v>
+      </c>
+      <c r="E44" t="s">
+        <v>182</v>
+      </c>
+      <c r="F44">
+        <v>0.56130000000000002</v>
+      </c>
+      <c r="G44">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H44">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>210</v>
+      </c>
+      <c r="B45">
+        <v>69</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <f>(100-B45)/100</f>
+        <v>0.31</v>
+      </c>
+      <c r="E45" t="s">
+        <v>182</v>
+      </c>
+      <c r="F45">
+        <v>0.74370000000000003</v>
+      </c>
+      <c r="G45">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H45">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>211</v>
+      </c>
+      <c r="B46">
+        <v>64</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <f>(100-B46)/100</f>
+        <v>0.36</v>
+      </c>
+      <c r="E46" t="s">
+        <v>182</v>
+      </c>
+      <c r="F46">
+        <v>0.7429</v>
+      </c>
+      <c r="G46">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H46">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>212</v>
+      </c>
+      <c r="B47">
+        <v>36</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <f>36/50</f>
+        <v>0.72</v>
+      </c>
+      <c r="E47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F47">
+        <v>0.77710000000000001</v>
+      </c>
+      <c r="G47">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H47">
+        <v>4.4400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A52" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B11">
-        <f>SUM(B2:B9)</f>
-        <v>0</v>
-      </c>
-      <c r="E11" t="e">
-        <f>AVERAGE(E2:E9)</f>
+      <c r="B52">
+        <f>SUM(B42:B50)</f>
+        <v>284</v>
+      </c>
+      <c r="C52">
+        <f>SUM(C42:C50)</f>
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <f>AVERAGE(D42:D48)</f>
+        <v>0.53999999999999992</v>
+      </c>
+      <c r="E52" t="e">
+        <f>AVERAGE(E42:E50)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F11">
-        <f>MAX(F2:F9)</f>
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f>MIN(G2:G9)</f>
-        <v>0</v>
+      <c r="F52">
+        <f>AVERAGE(F42:F50)</f>
+        <v>0.63035000000000008</v>
+      </c>
+      <c r="G52">
+        <f>MAX(G42:G50)</f>
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H52">
+        <f>MIN(H42:H50)</f>
+        <v>8.0000000000000007E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A55" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>215</v>
+      </c>
+      <c r="B56">
+        <v>52</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <f>(200-B56)/200</f>
+        <v>0.74</v>
+      </c>
+      <c r="E56" t="s">
+        <v>182</v>
+      </c>
+      <c r="F56">
+        <v>0.4279</v>
+      </c>
+      <c r="G56">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H56">
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>216</v>
+      </c>
+      <c r="B57">
+        <v>88</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <f>(200-B57)/200</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E57" t="s">
+        <v>182</v>
+      </c>
+      <c r="F57">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="G57">
+        <v>0.99970000000000003</v>
+      </c>
+      <c r="H57">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>217</v>
+      </c>
+      <c r="B58">
+        <v>79</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <f>(151-B58)/151</f>
+        <v>0.47682119205298013</v>
+      </c>
+      <c r="E58" t="s">
+        <v>182</v>
+      </c>
+      <c r="F58">
+        <v>0.64039999999999997</v>
+      </c>
+      <c r="G58">
+        <v>0.99939999999999996</v>
+      </c>
+      <c r="H58">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A60" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B60">
+        <f>SUM(B56:B58)</f>
+        <v>219</v>
+      </c>
+      <c r="C60">
+        <f>SUM(C56:C58)</f>
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <f>AVERAGE(D56:D58)</f>
+        <v>0.59227373068432676</v>
+      </c>
+      <c r="E60" t="e">
+        <f>AVERAGE(E56:E58)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F60">
+        <v>0.48</v>
+      </c>
+      <c r="G60">
+        <f>MAX(G56:G58)</f>
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H60">
+        <f>MIN(H56:H58)</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>215</v>
+      </c>
+      <c r="B63">
+        <v>196</v>
+      </c>
+      <c r="C63">
+        <v>196</v>
+      </c>
+      <c r="D63">
+        <f>196/200</f>
+        <v>0.98</v>
+      </c>
+      <c r="E63">
+        <f>196/200</f>
+        <v>0.98</v>
+      </c>
+      <c r="F63">
+        <v>0.97819999999999996</v>
+      </c>
+      <c r="G63">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H63">
+        <v>0.54510000000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>219</v>
+      </c>
+      <c r="B64">
+        <v>89</v>
+      </c>
+      <c r="C64">
+        <v>89</v>
+      </c>
+      <c r="D64">
+        <f>89/90</f>
+        <v>0.98888888888888893</v>
+      </c>
+      <c r="E64">
+        <f>89/90</f>
+        <v>0.98888888888888893</v>
+      </c>
+      <c r="F64">
+        <v>0.99229999999999996</v>
+      </c>
+      <c r="G64">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H64">
+        <v>0.74529999999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B67">
+        <f>SUM(B63:B65)</f>
+        <v>285</v>
+      </c>
+      <c r="C67">
+        <f>SUM(C63:C65)</f>
+        <v>285</v>
+      </c>
+      <c r="D67">
+        <f>AVERAGE(D63:D65)</f>
+        <v>0.98444444444444446</v>
+      </c>
+      <c r="E67">
+        <f>AVERAGE(E63:E65)</f>
+        <v>0.98444444444444446</v>
+      </c>
+      <c r="F67">
+        <f>AVERAGE(F63:F64)</f>
+        <v>0.98524999999999996</v>
+      </c>
+      <c r="G67">
+        <f>MAX(G63:G65)</f>
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H67">
+        <f>MIN(H63:H65)</f>
+        <v>0.54510000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>